<commit_message>
Added refecences to documentation
</commit_message>
<xml_diff>
--- a/harvesting/Docs/JoiningMIMOprocesses.xlsx
+++ b/harvesting/Docs/JoiningMIMOprocesses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Tasks</t>
   </si>
@@ -51,9 +51,6 @@
     <t>period 6</t>
   </si>
   <si>
-    <t>REMARKS</t>
-  </si>
-  <si>
     <t>IT Task : Send your LIDO records into a unique file (static OAI repository)</t>
   </si>
   <si>
@@ -85,6 +82,18 @@
   </si>
   <si>
     <t>Download and send  back the Content Checklist</t>
+  </si>
+  <si>
+    <t>REMARKS / additional info</t>
+  </si>
+  <si>
+    <t>SeeMIMO_Digitisation_Standard_v3.pdf</t>
+  </si>
+  <si>
+    <t>See Metadata_Mapping_And_OAI-PMH_implementation_guidelines.pdf &amp; Specification_of_the_data_model_for_musical_instruments.pdf &amp; MIMO_Thesaurus.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One high res image for the home page ; 5 preferred instruments with the corresponding Ids ; A short text describing your museum ; A logo of your instituion ( B&amp;W and colored version ) </t>
   </si>
 </sst>
 </file>
@@ -174,11 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -190,6 +197,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,155 +516,159 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.88671875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="70.88671875" style="11" customWidth="1"/>
     <col min="2" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="76.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="86.21875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>15</v>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
+      <c r="A4" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="2"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
+      <c r="I5" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
+      <c r="A7" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>18</v>
+      <c r="A8" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>12</v>
+      <c r="A9" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1"/>
@@ -650,12 +676,12 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="1"/>
@@ -664,14 +690,14 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>13</v>
+      <c r="H11" s="6"/>
+      <c r="I11" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -679,12 +705,14 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
+      <c r="A15" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>